<commit_message>
Initial version of visualizer functions and visualizer script; separated incomplete dataset
</commit_message>
<xml_diff>
--- a/data/Question_Topics.xlsx
+++ b/data/Question_Topics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikolay/Documents/UW/AUT22/CSE583/group_project/learning-with-python/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55DFE567-4B65-7647-8515-17323CA23907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47468B8-901A-9E45-A5BB-8A6D0FB10347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14800" yWindow="8820" windowWidth="26040" windowHeight="14940" xr2:uid="{A7347213-28CC-6444-A6DB-4FB61079D7FD}"/>
+    <workbookView xWindow="660" yWindow="1280" windowWidth="18260" windowHeight="20800" xr2:uid="{A7347213-28CC-6444-A6DB-4FB61079D7FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B22630C-8240-2940-A760-0E41631CF4AE}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="98" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>